<commit_message>
create local docker files for baking Ampersand images
In case RAP cannot wait for the latest release of Ampersand, these docker
files allow the developer to bake images from the development branch of
Ampersand.
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80A2168-9A0F-EE4F-A56A-DE3F177EFA50}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="11655" windowHeight="5340"/>
+    <workbookView xWindow="240" yWindow="440" windowWidth="17900" windowHeight="10340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>Organization</t>
   </si>
@@ -124,30 +125,12 @@
     <t>de</t>
   </si>
   <si>
-    <t>Debbie Tarenskeen</t>
-  </si>
-  <si>
-    <t>Debbie</t>
-  </si>
-  <si>
-    <t>Tarenskeen</t>
-  </si>
-  <si>
-    <t>HAN</t>
-  </si>
-  <si>
-    <t>Hogeschool Arnhem Nijmegen</t>
-  </si>
-  <si>
     <t>lloydr</t>
   </si>
   <si>
     <t>stefj</t>
   </si>
   <si>
-    <t>debbiet</t>
-  </si>
-  <si>
     <t>GradStudent</t>
   </si>
   <si>
@@ -178,21 +161,12 @@
     <t>estherh</t>
   </si>
   <si>
-    <t>rienh</t>
-  </si>
-  <si>
     <t>Acc_Esther</t>
   </si>
   <si>
-    <t>Acc_Rien</t>
-  </si>
-  <si>
     <t>Esther Hageraats</t>
   </si>
   <si>
-    <t>Rien Hamers</t>
-  </si>
-  <si>
     <t>Acc_Stef</t>
   </si>
   <si>
@@ -205,31 +179,19 @@
     <t>Acc_Jan</t>
   </si>
   <si>
-    <t>Acc_Debbie</t>
-  </si>
-  <si>
     <t>Esther</t>
   </si>
   <si>
     <t>Hageraats</t>
   </si>
   <si>
-    <t>Hamers</t>
-  </si>
-  <si>
-    <t>Rien</t>
-  </si>
-  <si>
     <t>Saxion</t>
-  </si>
-  <si>
-    <t>Fontys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +263,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -322,23 +284,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -354,9 +310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -394,9 +350,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -429,9 +385,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,9 +437,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -639,36 +629,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.1640625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2"/>
@@ -678,17 +667,17 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2"/>
@@ -698,36 +687,36 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
-        <f t="shared" ref="A5:A8" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
+        <f t="shared" ref="A5:A7" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van der Wetering</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -737,442 +726,348 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>64</v>
+        <v>49</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="str">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="str">
+        <f>IF($B10="","",$B10)</f>
+        <v>OUNL</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="str">
+        <f>IF($B15="","",CONCATENATE("Acc_",$B3))</f>
+        <v>Acc_Stef</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f>$A3</f>
+        <v>Stef Joosten</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f>$A$10</f>
+        <v>OUNL</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="str">
+        <f>IF($B16="","",CONCATENATE("Acc_",$B4))</f>
+        <v>Acc_Lloyd</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="7" t="str">
+        <f>$A4</f>
+        <v>Lloyd Rutledge</v>
+      </c>
+      <c r="E16" s="5" t="str">
+        <f t="shared" ref="E16:E19" si="2">$A$10</f>
+        <v>OUNL</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="str">
-        <f>IF($B12="","",$B12)</f>
+      <c r="J16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="str">
+        <f>IF($B17="","",CONCATENATE("Acc_",$B5))</f>
+        <v>Acc_Rogier</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f t="shared" ref="D17" si="3">$A5</f>
+        <v>Rogier van der Wetering</v>
+      </c>
+      <c r="E17" s="5" t="str">
+        <f t="shared" si="2"/>
         <v>OUNL</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="G17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="2" t="s">
+      <c r="E18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
-        <f>IF($B19="","",CONCATENATE("Acc_",$B3))</f>
-        <v>Acc_Stef</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>42</v>
+        <f>IF($B19="","",CONCATENATE("Acc_",$B7))</f>
+        <v>Acc_Jan</v>
+      </c>
+      <c r="B19" s="9">
+        <v>123456</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f>$A3</f>
-        <v>Stef Joosten</v>
+        <f>$A7</f>
+        <v>Jan de Student</v>
       </c>
       <c r="E19" s="5" t="str">
-        <f>$A$12</f>
-        <v>OUNL</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="str">
-        <f>IF($B20="","",CONCATENATE("Acc_",$B4))</f>
-        <v>Acc_Lloyd</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7" t="str">
-        <f>$A4</f>
-        <v>Lloyd Rutledge</v>
-      </c>
-      <c r="E20" s="5" t="str">
-        <f t="shared" ref="E20:E24" si="2">$A$12</f>
-        <v>OUNL</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="str">
-        <f>IF($B21="","",CONCATENATE("Acc_",$B5))</f>
-        <v>Acc_Rogier</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="7" t="str">
-        <f t="shared" ref="D21" si="3">$A5</f>
-        <v>Rogier van der Wetering</v>
-      </c>
-      <c r="E21" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OUNL</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="F19" s="3">
+        <v>123456</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="B22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="str">
-        <f>IF($B24="","",CONCATENATE("Acc_",$B8))</f>
-        <v>Acc_Jan</v>
-      </c>
-      <c r="B24" s="10">
-        <v>123456</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="7" t="str">
-        <f>$A8</f>
-        <v>Jan de Student</v>
-      </c>
-      <c r="E24" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>OUNL</v>
-      </c>
-      <c r="F24" s="3">
-        <v>123456</v>
-      </c>
-      <c r="G24" s="3" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="str">
-        <f>IF($B25="","",CONCATENATE("Acc_",$B9))</f>
-        <v>Acc_Debbie</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="5" t="str">
-        <f>$A$16</f>
-        <v>HAN</v>
-      </c>
-      <c r="F25"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B23" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>51</v>
+      <c r="B25" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make RAP3 build again with Michiel's multistage-build
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F04D67A-21B0-4A41-909F-CD4FC7275028}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C29E7E-B647-EF4E-82C2-9C2F249F0C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>Organization</t>
   </si>
@@ -184,9 +184,6 @@
     <t>rogiervdw</t>
   </si>
   <si>
-    <t>Acc_Esther</t>
-  </si>
-  <si>
     <t>Esther Hageraats</t>
   </si>
   <si>
@@ -215,13 +212,37 @@
   </si>
   <si>
     <t>Fontys</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>PF_Label</t>
+  </si>
+  <si>
+    <t>SystemAdmin</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Anonymous</t>
+  </si>
+  <si>
+    <t>ExecEngine</t>
+  </si>
+  <si>
+    <t>Janitor</t>
+  </si>
+  <si>
+    <t>SYSTEM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +264,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -292,7 +319,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -325,11 +352,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -345,7 +373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -665,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -763,13 +791,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -844,18 +872,18 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -971,7 +999,7 @@
         <v>44</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -990,7 +1018,7 @@
         <v>Lloyd Rutledge</v>
       </c>
       <c r="E19" s="5" t="str">
-        <f t="shared" ref="E19:E22" si="2">$A$11</f>
+        <f t="shared" ref="E19:E20" si="2">$A$11</f>
         <v>OUNL</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1003,7 +1031,7 @@
         <v>44</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1032,133 +1060,179 @@
         <v>51</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>54</v>
+      <c r="A21" s="6" t="str">
+        <f>IF($B21="","",CONCATENATE("Acc_",$B7))</f>
+        <v>Acc_Jan</v>
+      </c>
+      <c r="B21" s="10">
+        <v>123456</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="7" t="str">
+        <f>$A7</f>
+        <v>Jan de Student</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>62</v>
       </c>
+      <c r="F21" s="3">
+        <v>123456</v>
+      </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="str">
-        <f>IF($B22="","",CONCATENATE("Acc_",$B7))</f>
-        <v>Acc_Jan</v>
-      </c>
-      <c r="B22" s="10">
-        <v>123456</v>
-      </c>
-      <c r="C22" s="4" t="s">
+        <f>IF($B22="","",CONCATENATE("Acc_",$B8))</f>
+        <v>Acc_Debbie</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7" t="str">
-        <f>$A7</f>
-        <v>Jan de Student</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="3">
-        <v>12345</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>33</v>
+      <c r="D22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="5" t="str">
+        <f>$A$15</f>
+        <v>HAN</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="str">
-        <f>IF($B23="","",CONCATENATE("Acc_",$B8))</f>
-        <v>Acc_Debbie</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="5" t="str">
-        <f>$A$15</f>
-        <v>HAN</v>
-      </c>
-      <c r="F23"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>59</v>
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>47</v>
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>51</v>
+      <c r="A29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade to SIAMv4 for the login.
This version builds, but does not run properly yet.
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C29E7E-B647-EF4E-82C2-9C2F249F0C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F89C9C-B929-8C4A-9619-3FF4BE5140C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Organization</t>
   </si>
@@ -40,9 +40,6 @@
     <t>accPassword</t>
   </si>
   <si>
-    <t>UserID</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -103,24 +100,12 @@
     <t>Rogier</t>
   </si>
   <si>
-    <t>Wetering</t>
-  </si>
-  <si>
-    <t>personMiddle</t>
-  </si>
-  <si>
-    <t>van der</t>
-  </si>
-  <si>
     <t>OUNL</t>
   </si>
   <si>
     <t>Open Universiteit Nederland</t>
   </si>
   <si>
-    <t>Middlepart</t>
-  </si>
-  <si>
     <t>Jan</t>
   </si>
   <si>
@@ -130,9 +115,6 @@
     <t>Tutor</t>
   </si>
   <si>
-    <t>de</t>
-  </si>
-  <si>
     <t>Debbie Tarenskeen</t>
   </si>
   <si>
@@ -163,12 +145,6 @@
     <t>[Roles]</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>RoleName</t>
-  </si>
-  <si>
     <t>accIsActive</t>
   </si>
   <si>
@@ -236,13 +212,43 @@
   </si>
   <si>
     <t>SYSTEM</t>
+  </si>
+  <si>
+    <t>Userid</t>
+  </si>
+  <si>
+    <t>van de Wetering</t>
+  </si>
+  <si>
+    <t>Rogier.vandeWetering@ou.nl</t>
+  </si>
+  <si>
+    <t>de Student</t>
+  </si>
+  <si>
+    <t>isPartOf</t>
+  </si>
+  <si>
+    <t>[PF_NavMenuItem]</t>
+  </si>
+  <si>
+    <t>PF_NavMenuItem</t>
+  </si>
+  <si>
+    <t>PF_NavMenu</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +276,14 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -314,12 +328,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -353,9 +368,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -693,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -712,16 +731,14 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1" s="9"/>
       <c r="D1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -732,16 +749,14 @@
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -756,10 +771,10 @@
         <v>Stef Joosten</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -768,36 +783,36 @@
         <v>Lloyd Rutledge</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
         <f t="shared" ref="A5:A7" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
-        <v>Rogier van der Wetering</v>
+        <v>Rogier van de Wetering</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>64</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -806,35 +821,32 @@
         <v>Jan de Student</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="2"/>
@@ -864,48 +876,48 @@
         <v>OUNL</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -919,25 +931,23 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -945,26 +955,24 @@
         <v>2</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>2</v>
@@ -976,10 +984,10 @@
         <v>Acc_Stef</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="7" t="str">
         <f>$A3</f>
@@ -990,16 +998,16 @@
         <v>OUNL</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1008,10 +1016,10 @@
         <v>Acc_Lloyd</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="7" t="str">
         <f>$A4</f>
@@ -1022,16 +1030,16 @@
         <v>OUNL</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1040,27 +1048,27 @@
         <v>Acc_Rogier</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="7" t="str">
         <f t="shared" ref="D20" si="3">$A5</f>
-        <v>Rogier van der Wetering</v>
+        <v>Rogier van de Wetering</v>
       </c>
       <c r="E20" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OUNL</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1072,23 +1080,20 @@
         <v>123456</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="7" t="str">
         <f>$A7</f>
         <v>Jan de Student</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="3">
-        <v>123456</v>
+        <v>54</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1097,13 +1102,13 @@
         <v>Acc_Debbie</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E22" s="5" t="str">
         <f>$A$15</f>
@@ -1112,131 +1117,162 @@
       <c r="F22"/>
       <c r="G22" s="8"/>
       <c r="H22" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>46</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>47</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="B37" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>70</v>
+      <c r="C38" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{E3E2B40F-D1BD-E142-BA42-403812FCF30B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying to get compile-buttons to work with Ampersand 4.0.0
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874D58FE-9273-DC48-A83F-0A5C4573FF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A831B-844B-BB4F-B7B7-AF013D430DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>Organization</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>welkom01</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>FormalAmpersand</t>
+  </si>
+  <si>
+    <t>Type_32_Checker</t>
   </si>
 </sst>
 </file>
@@ -712,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1145,9 @@
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="C23" s="9" t="s">
         <v>53</v>
       </c>
@@ -1139,7 +1156,9 @@
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="C24" s="9" t="s">
         <v>54</v>
       </c>
@@ -1148,6 +1167,9 @@
       <c r="A25" t="s">
         <v>28</v>
       </c>
+      <c r="B25" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="C25" s="10" t="s">
         <v>28</v>
       </c>
@@ -1156,6 +1178,9 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
+      <c r="B26" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="C26" s="10" t="s">
         <v>27</v>
       </c>
@@ -1164,6 +1189,9 @@
       <c r="A27" t="s">
         <v>36</v>
       </c>
+      <c r="B27" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="C27" s="10" t="s">
         <v>36</v>
       </c>
@@ -1172,6 +1200,9 @@
       <c r="A28" t="s">
         <v>41</v>
       </c>
+      <c r="B28" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C28" s="10" t="s">
         <v>41</v>
       </c>
@@ -1180,6 +1211,9 @@
       <c r="A29" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="B29" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C29" s="12" t="s">
         <v>55</v>
       </c>
@@ -1188,6 +1222,9 @@
       <c r="A30" s="12" t="s">
         <v>56</v>
       </c>
+      <c r="B30" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="C30" s="12" t="s">
         <v>56</v>
       </c>
@@ -1196,6 +1233,9 @@
       <c r="A31" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="B31" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="C31" s="12" t="s">
         <v>57</v>
       </c>
@@ -1204,6 +1244,9 @@
       <c r="A32" s="12" t="s">
         <v>58</v>
       </c>
+      <c r="B32" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="C32" s="12" t="s">
         <v>58</v>
       </c>
@@ -1212,6 +1255,9 @@
       <c r="A33" s="12" t="s">
         <v>59</v>
       </c>
+      <c r="B33" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="C33" s="12" t="s">
         <v>59</v>
       </c>
@@ -1220,51 +1266,81 @@
       <c r="A34" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="B34" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="C34" s="12" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="12"/>
+    </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>69</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C37" s="12"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B43" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make Atlas work more user-friendly
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A831B-844B-BB4F-B7B7-AF013D430DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DE72E7-A830-464A-AD7B-8FBCC856BB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -730,7 +730,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="B23" sqref="B23:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Bugfix missing label for 3 roles
</commit_message>
<xml_diff>
--- a/RAP3/src/RAP3.xlsx
+++ b/RAP3/src/RAP3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B905994C-CA8E-8E4B-9F2D-43DB68DA4EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA2C5E2-ADE2-4F5E-A4CC-47CF8CDA9DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="29520" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Identity Provider data" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>Organization</t>
   </si>
@@ -242,13 +242,16 @@
   </si>
   <si>
     <t>welkom</t>
+  </si>
+  <si>
+    <t>Type Checker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,10 +373,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Berekening" xfId="2" builtinId="22"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -389,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -711,22 +714,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.1640625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -743,7 +746,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -760,7 +763,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="7" t="str">
         <f t="shared" ref="A3" si="0">IF($B3="","",CONCATENATE($B3," ",IF($C3="",D3,CONCATENATE($C3," ",$D3))))</f>
         <v>Stef Joosten</v>
@@ -772,7 +775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="7" t="str">
         <f>IF($B4="","",CONCATENATE($B4," ",IF($C4="",D4,CONCATENATE($C4," ",$D4))))</f>
         <v>Lloyd Rutledge</v>
@@ -784,7 +787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="str">
         <f t="shared" ref="A5:A6" si="1">IF($B5="","",CONCATENATE($B5," ",IF($C5="",D5,CONCATENATE($C5," ",$D5))))</f>
         <v>Rogier van de Wetering</v>
@@ -799,7 +802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Jan de Student</v>
@@ -811,7 +814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -822,7 +825,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -839,7 +842,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +855,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="7" t="str">
         <f>IF($B10="","",$B10)</f>
         <v>OUNL</v>
@@ -864,7 +867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -872,7 +875,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -880,7 +883,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -891,7 +894,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
@@ -902,7 +905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="1" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -929,7 +932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -954,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="6" t="str">
         <f>IF($B17="","",CONCATENATE("Acc_",$B3))</f>
         <v>Acc_Stef</v>
@@ -983,7 +986,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="6" t="str">
         <f>IF($B18="","",CONCATENATE("Acc_",$B4))</f>
         <v>Acc_Lloyd</v>
@@ -1012,7 +1015,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="6" t="str">
         <f>IF($B19="","",CONCATENATE("Acc_",$B5))</f>
         <v>Acc_Rogier</v>
@@ -1038,7 +1041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="6" t="str">
         <f>IF($B20="","",CONCATENATE("Acc_",$B6))</f>
         <v>Acc_Jan</v>
@@ -1060,7 +1063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="6" t="str">
         <f>IF($B21="","",CONCATENATE("Acc_",$B7))</f>
         <v>Acc_Debbie</v>
@@ -1087,7 +1090,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="11" t="s">
         <v>50</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="11" t="s">
         <v>51</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="11" t="s">
         <v>52</v>
       </c>
@@ -1164,7 +1167,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="11" t="s">
         <v>53</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="11" t="s">
         <v>54</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="11" t="s">
         <v>55</v>
       </c>
@@ -1197,34 +1200,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
         <v>61</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="11" t="s">
         <v>62</v>
       </c>
@@ -1246,7 +1255,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="11" t="s">
         <v>64</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="11" t="s">
         <v>65</v>
       </c>

</xml_diff>